<commit_message>
Include many products in the same invoice
</commit_message>
<xml_diff>
--- a/spreadsheet/template.xlsx
+++ b/spreadsheet/template.xlsx
@@ -60,9 +60,6 @@
     <t xml:space="preserve">Remote controllers</t>
   </si>
   <si>
-    <t>20,50</t>
-  </si>
-  <si>
     <t>2021-000002</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dulce de leche 1kg.</t>
+  </si>
+  <si>
+    <t>Waffles</t>
   </si>
 </sst>
 </file>
@@ -726,31 +726,31 @@
       <c r="H2" s="2">
         <v>250</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>15</v>
+      <c r="I2" s="3">
+        <v>20.5</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
       <c r="F3">
         <v>800045</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>45</v>
@@ -761,31 +761,46 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
       </c>
       <c r="F4">
         <v>33446685</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>125</v>
       </c>
       <c r="I4">
         <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>250</v>
+      </c>
+      <c r="I5">
+        <v>2.3999999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>